<commit_message>
Resultados do beachmark com outros sistemas
</commit_message>
<xml_diff>
--- a/Spec/benchmark_results/Detalhado/ElectricDevices.xlsx
+++ b/Spec/benchmark_results/Detalhado/ElectricDevices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\Projeto\Experimentos\Spec\Spec\benchmark_results\Detalhado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA1F8FC-0E39-45F2-8BA8-CCD3CE6339B8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34940EB-BB46-49BB-ADFF-92A94F668651}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -85,157 +85,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="142" x14ac:knownFonts="1">
+  <fonts count="114" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
@@ -853,7 +709,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="142">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -983,39 +839,7 @@
     <xf numFmtId="0" fontId="110" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="111" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="112" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="113" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="114" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="115" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="116" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="117" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="118" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="119" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="120" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="121" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="122" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="123" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="124" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="125" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="126" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="127" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="128" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="129" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="130" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="131" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="132" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="133" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="134" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="135" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="136" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="137" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="138" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="139" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="140" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="141" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="113" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1424,31 +1248,31 @@
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="141">
+      <c r="H3" s="113">
         <f t="shared" ref="H3:N3" si="0">AVERAGE(H2)</f>
         <v>0</v>
       </c>
-      <c r="I3" s="141">
+      <c r="I3" s="113">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="J3" s="141">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K3" s="141">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L3" s="141">
+      <c r="J3" s="113">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K3" s="113">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L3" s="113">
         <f t="shared" si="0"/>
         <v>0.17391304347826086</v>
       </c>
-      <c r="M3" s="141">
+      <c r="M3" s="113">
         <f t="shared" si="0"/>
         <v>2.1739130434782608E-2</v>
       </c>
-      <c r="N3" s="141">
+      <c r="N3" s="113">
         <f t="shared" si="0"/>
         <v>-4.4399596367305748E-2</v>
       </c>
@@ -1477,81 +1301,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C1" s="128" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="128" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="128" t="s">
+      <c r="C1" s="100" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="100" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="100" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="128" t="s">
+      <c r="F1" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="128" t="s">
+      <c r="G1" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="128" t="s">
+      <c r="H1" s="100" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="128" t="s">
+      <c r="I1" s="100" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="128" t="s">
+      <c r="J1" s="100" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="128" t="s">
+      <c r="K1" s="100" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="128" t="s">
+      <c r="L1" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="128" t="s">
+      <c r="M1" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="128" t="s">
+      <c r="N1" s="100" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="127" t="s">
+      <c r="B2" s="99" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="129">
+      <c r="C2" s="101">
         <v>44</v>
       </c>
-      <c r="D2" s="130">
-        <v>1</v>
-      </c>
-      <c r="E2" s="131">
-        <v>1</v>
-      </c>
-      <c r="F2" s="132">
+      <c r="D2" s="102">
+        <v>1</v>
+      </c>
+      <c r="E2" s="103">
+        <v>1</v>
+      </c>
+      <c r="F2" s="104">
         <v>56</v>
       </c>
-      <c r="G2" s="133">
+      <c r="G2" s="105">
         <v>43</v>
       </c>
-      <c r="H2" s="134">
+      <c r="H2" s="106">
         <v>2.2727272727272728E-2</v>
       </c>
-      <c r="I2" s="135">
+      <c r="I2" s="107">
         <v>1.7543859649122806E-2</v>
       </c>
-      <c r="J2" s="136">
+      <c r="J2" s="108">
         <v>1.7543859649122806E-2</v>
       </c>
-      <c r="K2" s="137">
+      <c r="K2" s="109">
         <v>1.9801980198019802E-2</v>
       </c>
-      <c r="L2" s="138">
+      <c r="L2" s="110">
         <v>1.9049273348387474E-2</v>
       </c>
-      <c r="M2" s="139">
+      <c r="M2" s="111">
         <v>1.9801980198019802E-2</v>
       </c>
-      <c r="N2" s="140">
+      <c r="N2" s="112">
         <v>-0.92844744455159101</v>
       </c>
     </row>
@@ -1559,31 +1383,31 @@
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="141">
+      <c r="H3" s="113">
         <f t="shared" ref="H3:N3" si="0">AVERAGE(H2)</f>
         <v>2.2727272727272728E-2</v>
       </c>
-      <c r="I3" s="141">
+      <c r="I3" s="113">
         <f t="shared" si="0"/>
         <v>1.7543859649122806E-2</v>
       </c>
-      <c r="J3" s="141">
+      <c r="J3" s="113">
         <f t="shared" si="0"/>
         <v>1.7543859649122806E-2</v>
       </c>
-      <c r="K3" s="141">
+      <c r="K3" s="113">
         <f t="shared" si="0"/>
         <v>1.9801980198019802E-2</v>
       </c>
-      <c r="L3" s="141">
+      <c r="L3" s="113">
         <f t="shared" si="0"/>
         <v>1.9049273348387474E-2</v>
       </c>
-      <c r="M3" s="141">
+      <c r="M3" s="113">
         <f t="shared" si="0"/>
         <v>1.9801980198019802E-2</v>
       </c>
-      <c r="N3" s="141">
+      <c r="N3" s="113">
         <f t="shared" si="0"/>
         <v>-0.92844744455159101</v>
       </c>
@@ -1694,31 +1518,31 @@
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="141">
+      <c r="H3" s="113">
         <f t="shared" ref="H3:N3" si="0">AVERAGE(H2)</f>
         <v>0</v>
       </c>
-      <c r="I3" s="141">
+      <c r="I3" s="113">
         <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="J3" s="141">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K3" s="141">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L3" s="141">
+      <c r="J3" s="113">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K3" s="113">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L3" s="113">
         <f t="shared" si="0"/>
         <v>6.2222222222222213E-2</v>
       </c>
-      <c r="M3" s="141">
+      <c r="M3" s="113">
         <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
-      <c r="N3" s="141">
+      <c r="N3" s="113">
         <f t="shared" si="0"/>
         <v>-0.21890547263681592</v>
       </c>
@@ -1829,31 +1653,31 @@
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="141">
+      <c r="H3" s="113">
         <f t="shared" ref="H3:N3" si="0">AVERAGE(H2)</f>
         <v>6.8181818181818177E-2</v>
       </c>
-      <c r="I3" s="141">
+      <c r="I3" s="113">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="J3" s="141">
+      <c r="J3" s="113">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="K3" s="141">
+      <c r="K3" s="113">
         <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
-      <c r="L3" s="141">
+      <c r="L3" s="113">
         <f t="shared" si="0"/>
         <v>0.23731884057971012</v>
       </c>
-      <c r="M3" s="141">
+      <c r="M3" s="113">
         <f t="shared" si="0"/>
         <v>8.6956521739130432E-2</v>
       </c>
-      <c r="N3" s="141">
+      <c r="N3" s="113">
         <f t="shared" si="0"/>
         <v>-4.0948275862068978E-2</v>
       </c>
@@ -1873,7 +1697,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="N3" sqref="B1:N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1964,31 +1788,31 @@
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="141">
+      <c r="H3" s="113">
         <f t="shared" ref="H3:N3" si="0">AVERAGE(H2)</f>
         <v>0.45454545454545453</v>
       </c>
-      <c r="I3" s="141">
+      <c r="I3" s="113">
         <f t="shared" si="0"/>
         <v>3.4482758620689655E-3</v>
       </c>
-      <c r="J3" s="141">
+      <c r="J3" s="113">
         <f t="shared" si="0"/>
         <v>6.4724919093851127E-2</v>
       </c>
-      <c r="K3" s="141">
+      <c r="K3" s="113">
         <f t="shared" si="0"/>
         <v>0.11331444759206799</v>
       </c>
-      <c r="L3" s="141">
+      <c r="L3" s="113">
         <f t="shared" si="0"/>
         <v>5.9878991650380985E-2</v>
       </c>
-      <c r="M3" s="141">
+      <c r="M3" s="113">
         <f t="shared" si="0"/>
         <v>6.2874251497005984E-2</v>
       </c>
-      <c r="N3" s="141">
+      <c r="N3" s="113">
         <f t="shared" si="0"/>
         <v>-0.15248594421783707</v>
       </c>
@@ -2008,7 +1832,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2017,115 +1841,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C1" s="58" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="58" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="58" t="s">
+      <c r="C1" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="58" t="s">
+      <c r="F1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="58" t="s">
+      <c r="G1" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="58" t="s">
+      <c r="H1" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="58" t="s">
+      <c r="I1" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="58" t="s">
+      <c r="J1" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="58" t="s">
+      <c r="K1" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="58" t="s">
+      <c r="L1" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="58" t="s">
+      <c r="M1" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="58" t="s">
+      <c r="N1" s="44" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="59">
+      <c r="C2" s="45">
         <v>44</v>
       </c>
-      <c r="D2" s="60">
-        <v>0</v>
-      </c>
-      <c r="E2" s="61">
-        <v>0</v>
-      </c>
-      <c r="F2" s="62">
-        <v>26</v>
-      </c>
-      <c r="G2" s="63">
-        <v>44</v>
-      </c>
-      <c r="H2" s="64">
-        <v>0</v>
-      </c>
-      <c r="I2" s="65">
-        <v>0</v>
-      </c>
-      <c r="J2" s="66">
-        <v>0</v>
-      </c>
-      <c r="K2" s="67">
-        <v>0</v>
-      </c>
-      <c r="L2" s="68">
-        <v>0</v>
-      </c>
-      <c r="M2" s="69">
-        <v>0</v>
-      </c>
-      <c r="N2" s="70">
-        <v>-0.87595712098009193</v>
+      <c r="D2" s="46">
+        <v>20</v>
+      </c>
+      <c r="E2" s="47">
+        <v>1</v>
+      </c>
+      <c r="F2" s="48">
+        <v>289</v>
+      </c>
+      <c r="G2" s="49">
+        <v>24</v>
+      </c>
+      <c r="H2" s="50">
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="I2" s="51">
+        <v>3.4482758620689655E-3</v>
+      </c>
+      <c r="J2" s="52">
+        <v>6.4724919093851127E-2</v>
+      </c>
+      <c r="K2" s="53">
+        <v>0.11331444759206799</v>
+      </c>
+      <c r="L2" s="54">
+        <v>5.9878991650380985E-2</v>
+      </c>
+      <c r="M2" s="55">
+        <v>6.2874251497005984E-2</v>
+      </c>
+      <c r="N2" s="56">
+        <v>-0.15248594421783707</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="141">
+      <c r="H3" s="113">
         <f t="shared" ref="H3:N3" si="0">AVERAGE(H2)</f>
-        <v>0</v>
-      </c>
-      <c r="I3" s="141">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J3" s="141">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K3" s="141">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L3" s="141">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M3" s="141">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N3" s="141">
-        <f t="shared" si="0"/>
-        <v>-0.87595712098009193</v>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="I3" s="113">
+        <f t="shared" si="0"/>
+        <v>3.4482758620689655E-3</v>
+      </c>
+      <c r="J3" s="113">
+        <f t="shared" si="0"/>
+        <v>6.4724919093851127E-2</v>
+      </c>
+      <c r="K3" s="113">
+        <f t="shared" si="0"/>
+        <v>0.11331444759206799</v>
+      </c>
+      <c r="L3" s="113">
+        <f t="shared" si="0"/>
+        <v>5.9878991650380985E-2</v>
+      </c>
+      <c r="M3" s="113">
+        <f t="shared" si="0"/>
+        <v>6.2874251497005984E-2</v>
+      </c>
+      <c r="N3" s="113">
+        <f t="shared" si="0"/>
+        <v>-0.15248594421783707</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -2143,7 +1967,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2152,115 +1976,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C1" s="72" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="72" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="72" t="s">
+      <c r="C1" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="72" t="s">
+      <c r="F1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="72" t="s">
+      <c r="G1" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="72" t="s">
+      <c r="H1" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="72" t="s">
+      <c r="I1" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="72" t="s">
+      <c r="J1" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="72" t="s">
+      <c r="K1" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="72" t="s">
+      <c r="L1" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="72" t="s">
+      <c r="M1" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="72" t="s">
+      <c r="N1" s="44" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="73">
+      <c r="C2" s="45">
         <v>44</v>
       </c>
-      <c r="D2" s="74">
-        <v>0</v>
-      </c>
-      <c r="E2" s="75">
-        <v>1</v>
-      </c>
-      <c r="F2" s="76">
-        <v>0</v>
-      </c>
-      <c r="G2" s="77">
-        <v>44</v>
-      </c>
-      <c r="H2" s="78">
-        <v>0</v>
-      </c>
-      <c r="I2" s="79">
-        <v>1</v>
-      </c>
-      <c r="J2" s="80">
-        <v>0</v>
-      </c>
-      <c r="K2" s="81">
-        <v>0</v>
-      </c>
-      <c r="L2" s="82">
-        <v>0.34074074074074073</v>
-      </c>
-      <c r="M2" s="83">
-        <v>2.2222222222222223E-2</v>
-      </c>
-      <c r="N2" s="84">
-        <v>0</v>
+      <c r="D2" s="46">
+        <v>20</v>
+      </c>
+      <c r="E2" s="47">
+        <v>1</v>
+      </c>
+      <c r="F2" s="48">
+        <v>289</v>
+      </c>
+      <c r="G2" s="49">
+        <v>24</v>
+      </c>
+      <c r="H2" s="50">
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="I2" s="51">
+        <v>3.4482758620689655E-3</v>
+      </c>
+      <c r="J2" s="52">
+        <v>6.4724919093851127E-2</v>
+      </c>
+      <c r="K2" s="53">
+        <v>0.11331444759206799</v>
+      </c>
+      <c r="L2" s="54">
+        <v>5.9878991650380985E-2</v>
+      </c>
+      <c r="M2" s="55">
+        <v>6.2874251497005984E-2</v>
+      </c>
+      <c r="N2" s="56">
+        <v>-0.15248594421783707</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="141">
+      <c r="H3" s="113">
         <f t="shared" ref="H3:N3" si="0">AVERAGE(H2)</f>
-        <v>0</v>
-      </c>
-      <c r="I3" s="141">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J3" s="141">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K3" s="141">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L3" s="141">
-        <f t="shared" si="0"/>
-        <v>0.34074074074074073</v>
-      </c>
-      <c r="M3" s="141">
-        <f t="shared" si="0"/>
-        <v>2.2222222222222223E-2</v>
-      </c>
-      <c r="N3" s="141">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="I3" s="113">
+        <f t="shared" si="0"/>
+        <v>3.4482758620689655E-3</v>
+      </c>
+      <c r="J3" s="113">
+        <f t="shared" si="0"/>
+        <v>6.4724919093851127E-2</v>
+      </c>
+      <c r="K3" s="113">
+        <f t="shared" si="0"/>
+        <v>0.11331444759206799</v>
+      </c>
+      <c r="L3" s="113">
+        <f t="shared" si="0"/>
+        <v>5.9878991650380985E-2</v>
+      </c>
+      <c r="M3" s="113">
+        <f t="shared" si="0"/>
+        <v>6.2874251497005984E-2</v>
+      </c>
+      <c r="N3" s="113">
+        <f t="shared" si="0"/>
+        <v>-0.15248594421783707</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -2287,81 +2111,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C1" s="86" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="86" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="86" t="s">
+      <c r="C1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="86" t="s">
+      <c r="F1" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="86" t="s">
+      <c r="G1" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="86" t="s">
+      <c r="H1" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="86" t="s">
+      <c r="I1" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="86" t="s">
+      <c r="J1" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="86" t="s">
+      <c r="K1" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="86" t="s">
+      <c r="L1" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="86" t="s">
+      <c r="M1" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="86" t="s">
+      <c r="N1" s="58" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="87">
+      <c r="C2" s="59">
         <v>44</v>
       </c>
-      <c r="D2" s="88">
-        <v>1</v>
-      </c>
-      <c r="E2" s="89">
-        <v>1</v>
-      </c>
-      <c r="F2" s="90">
+      <c r="D2" s="60">
+        <v>1</v>
+      </c>
+      <c r="E2" s="61">
+        <v>1</v>
+      </c>
+      <c r="F2" s="62">
         <v>7</v>
       </c>
-      <c r="G2" s="91">
+      <c r="G2" s="63">
         <v>43</v>
       </c>
-      <c r="H2" s="92">
+      <c r="H2" s="64">
         <v>2.2727272727272728E-2</v>
       </c>
-      <c r="I2" s="93">
+      <c r="I2" s="65">
         <v>0.125</v>
       </c>
-      <c r="J2" s="94">
+      <c r="J2" s="66">
         <v>0.125</v>
       </c>
-      <c r="K2" s="95">
+      <c r="K2" s="67">
         <v>3.8461538461538464E-2</v>
       </c>
-      <c r="L2" s="96">
+      <c r="L2" s="68">
         <v>6.7307692307692304E-2</v>
       </c>
-      <c r="M2" s="97">
+      <c r="M2" s="69">
         <v>3.8461538461538464E-2</v>
       </c>
-      <c r="N2" s="98">
+      <c r="N2" s="70">
         <v>-0.3</v>
       </c>
     </row>
@@ -2369,31 +2193,31 @@
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="141">
+      <c r="H3" s="113">
         <f t="shared" ref="H3:N3" si="0">AVERAGE(H2)</f>
         <v>2.2727272727272728E-2</v>
       </c>
-      <c r="I3" s="141">
+      <c r="I3" s="113">
         <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
-      <c r="J3" s="141">
+      <c r="J3" s="113">
         <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
-      <c r="K3" s="141">
+      <c r="K3" s="113">
         <f t="shared" si="0"/>
         <v>3.8461538461538464E-2</v>
       </c>
-      <c r="L3" s="141">
+      <c r="L3" s="113">
         <f t="shared" si="0"/>
         <v>6.7307692307692304E-2</v>
       </c>
-      <c r="M3" s="141">
+      <c r="M3" s="113">
         <f t="shared" si="0"/>
         <v>3.8461538461538464E-2</v>
       </c>
-      <c r="N3" s="141">
+      <c r="N3" s="113">
         <f t="shared" si="0"/>
         <v>-0.3</v>
       </c>
@@ -2422,81 +2246,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C1" s="100" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="100" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="100" t="s">
+      <c r="C1" s="72" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="100" t="s">
+      <c r="F1" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="100" t="s">
+      <c r="G1" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="100" t="s">
+      <c r="H1" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="100" t="s">
+      <c r="I1" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="100" t="s">
+      <c r="J1" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="100" t="s">
+      <c r="K1" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="100" t="s">
+      <c r="L1" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="100" t="s">
+      <c r="M1" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="100" t="s">
+      <c r="N1" s="72" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="101">
+      <c r="C2" s="73">
         <v>44</v>
       </c>
-      <c r="D2" s="102">
-        <v>0</v>
-      </c>
-      <c r="E2" s="103">
-        <v>1</v>
-      </c>
-      <c r="F2" s="104">
-        <v>0</v>
-      </c>
-      <c r="G2" s="105">
+      <c r="D2" s="74">
+        <v>0</v>
+      </c>
+      <c r="E2" s="75">
+        <v>1</v>
+      </c>
+      <c r="F2" s="76">
+        <v>0</v>
+      </c>
+      <c r="G2" s="77">
         <v>44</v>
       </c>
-      <c r="H2" s="106">
-        <v>0</v>
-      </c>
-      <c r="I2" s="107">
-        <v>1</v>
-      </c>
-      <c r="J2" s="108">
-        <v>0</v>
-      </c>
-      <c r="K2" s="109">
-        <v>0</v>
-      </c>
-      <c r="L2" s="110">
+      <c r="H2" s="78">
+        <v>0</v>
+      </c>
+      <c r="I2" s="79">
+        <v>1</v>
+      </c>
+      <c r="J2" s="80">
+        <v>0</v>
+      </c>
+      <c r="K2" s="81">
+        <v>0</v>
+      </c>
+      <c r="L2" s="82">
         <v>0.34074074074074073</v>
       </c>
-      <c r="M2" s="111">
+      <c r="M2" s="83">
         <v>2.2222222222222223E-2</v>
       </c>
-      <c r="N2" s="112">
+      <c r="N2" s="84">
         <v>0</v>
       </c>
     </row>
@@ -2504,31 +2328,31 @@
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="141">
+      <c r="H3" s="113">
         <f t="shared" ref="H3:N3" si="0">AVERAGE(H2)</f>
         <v>0</v>
       </c>
-      <c r="I3" s="141">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J3" s="141">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K3" s="141">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L3" s="141">
+      <c r="I3" s="113">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J3" s="113">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K3" s="113">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L3" s="113">
         <f t="shared" si="0"/>
         <v>0.34074074074074073</v>
       </c>
-      <c r="M3" s="141">
+      <c r="M3" s="113">
         <f t="shared" si="0"/>
         <v>2.2222222222222223E-2</v>
       </c>
-      <c r="N3" s="141">
+      <c r="N3" s="113">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2557,81 +2381,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C1" s="114" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="114" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="114" t="s">
+      <c r="C1" s="86" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="86" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="114" t="s">
+      <c r="F1" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="114" t="s">
+      <c r="G1" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="114" t="s">
+      <c r="H1" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="114" t="s">
+      <c r="I1" s="86" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="114" t="s">
+      <c r="J1" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="114" t="s">
+      <c r="K1" s="86" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="114" t="s">
+      <c r="L1" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="114" t="s">
+      <c r="M1" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="114" t="s">
+      <c r="N1" s="86" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="113" t="s">
+      <c r="B2" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="115">
+      <c r="C2" s="87">
         <v>44</v>
       </c>
-      <c r="D2" s="116">
-        <v>0</v>
-      </c>
-      <c r="E2" s="117">
-        <v>1</v>
-      </c>
-      <c r="F2" s="118">
-        <v>1</v>
-      </c>
-      <c r="G2" s="119">
+      <c r="D2" s="88">
+        <v>0</v>
+      </c>
+      <c r="E2" s="89">
+        <v>1</v>
+      </c>
+      <c r="F2" s="90">
+        <v>1</v>
+      </c>
+      <c r="G2" s="91">
         <v>44</v>
       </c>
-      <c r="H2" s="120">
-        <v>0</v>
-      </c>
-      <c r="I2" s="121">
+      <c r="H2" s="92">
+        <v>0</v>
+      </c>
+      <c r="I2" s="93">
         <v>0.5</v>
       </c>
-      <c r="J2" s="122">
-        <v>0</v>
-      </c>
-      <c r="K2" s="123">
-        <v>0</v>
-      </c>
-      <c r="L2" s="124">
+      <c r="J2" s="94">
+        <v>0</v>
+      </c>
+      <c r="K2" s="95">
+        <v>0</v>
+      </c>
+      <c r="L2" s="96">
         <v>0.17391304347826086</v>
       </c>
-      <c r="M2" s="125">
+      <c r="M2" s="97">
         <v>2.1739130434782608E-2</v>
       </c>
-      <c r="N2" s="126">
+      <c r="N2" s="98">
         <v>-4.4399596367305748E-2</v>
       </c>
     </row>
@@ -2639,31 +2463,31 @@
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="141">
+      <c r="H3" s="113">
         <f t="shared" ref="H3:N3" si="0">AVERAGE(H2)</f>
         <v>0</v>
       </c>
-      <c r="I3" s="141">
+      <c r="I3" s="113">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="J3" s="141">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K3" s="141">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L3" s="141">
+      <c r="J3" s="113">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K3" s="113">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L3" s="113">
         <f t="shared" si="0"/>
         <v>0.17391304347826086</v>
       </c>
-      <c r="M3" s="141">
+      <c r="M3" s="113">
         <f t="shared" si="0"/>
         <v>2.1739130434782608E-2</v>
       </c>
-      <c r="N3" s="141">
+      <c r="N3" s="113">
         <f t="shared" si="0"/>
         <v>-4.4399596367305748E-2</v>
       </c>

</xml_diff>